<commit_message>
Updated availability till 27/01/23
</commit_message>
<xml_diff>
--- a/Daily calendar.xlsx
+++ b/Daily calendar.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F1E7B9-D988-4B4D-8FB0-437FEC3AB64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{012957D2-1B67-D245-8F1B-BC17252E38B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wk 1 (20-22 Jan)" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
     <numFmt numFmtId="166" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
     <numFmt numFmtId="167" formatCode="[$-809]dd\ mmmm\ yyyy\,\ dddd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -190,6 +190,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -254,7 +261,7 @@
     </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -303,6 +310,21 @@
     <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Date" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -312,7 +334,82 @@
     <cellStyle name="Time" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="156">
+  <dxfs count="159">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4177,10 +4274,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Daily Appointment Calendar" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Daily Appointment Calendar" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="155"/>
-      <tableStyleElement type="headerRow" dxfId="154"/>
-      <tableStyleElement type="totalRow" dxfId="153"/>
-      <tableStyleElement type="firstRowStripe" dxfId="152"/>
+      <tableStyleElement type="wholeTable" dxfId="158"/>
+      <tableStyleElement type="headerRow" dxfId="157"/>
+      <tableStyleElement type="totalRow" dxfId="156"/>
+      <tableStyleElement type="firstRowStripe" dxfId="155"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4207,10 +4304,10 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{9D17AAE6-FB8C-4478-A34D-2A51B6628A71}" name="Oksana" dataDxfId="151"/>
-    <tableColumn id="4" xr3:uid="{A9C8FF4C-AD28-4094-882D-B25729BB2D4B}" name="Yash" dataDxfId="150" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{C328F71A-BA70-4E02-9707-7A3FCE2EED0B}" name="Shin" dataDxfId="149"/>
-    <tableColumn id="8" xr3:uid="{F9054911-3417-4C55-A57F-3697BCFB4591}" name="Singapore time _x000a_(UTC+8)" dataDxfId="148" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{9D17AAE6-FB8C-4478-A34D-2A51B6628A71}" name="Oksana" dataDxfId="154"/>
+    <tableColumn id="4" xr3:uid="{A9C8FF4C-AD28-4094-882D-B25729BB2D4B}" name="Yash" dataDxfId="153" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{C328F71A-BA70-4E02-9707-7A3FCE2EED0B}" name="Shin" dataDxfId="152"/>
+    <tableColumn id="8" xr3:uid="{F9054911-3417-4C55-A57F-3697BCFB4591}" name="Singapore time _x000a_(UTC+8)" dataDxfId="151" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4229,10 +4326,10 @@
     <tableColumn id="2" xr3:uid="{CF6C4F92-C8BF-4216-8625-48CE0829E21D}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{82F93066-79A2-4BDD-86AC-57C0EA7C996B}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{1AC0FEC9-DD89-4B28-82F3-9DD705AA970C}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{EA5E7E24-5DE4-4CCC-8A86-B8199725346B}" name="Oksana" dataDxfId="115"/>
-    <tableColumn id="4" xr3:uid="{DF234A86-F25C-42D8-BC0F-F984E484C9BE}" name="Yash" dataDxfId="114" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{E153EC59-EC37-4ED1-887B-2680986E3BE3}" name="Shin" dataDxfId="113"/>
-    <tableColumn id="8" xr3:uid="{D548D9A8-FE15-481F-BAC8-E7E1A689769D}" name="Singapore time _x000a_(UTC+8)" dataDxfId="112" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{EA5E7E24-5DE4-4CCC-8A86-B8199725346B}" name="Oksana" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{DF234A86-F25C-42D8-BC0F-F984E484C9BE}" name="Yash" dataDxfId="117" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{E153EC59-EC37-4ED1-887B-2680986E3BE3}" name="Shin" dataDxfId="116"/>
+    <tableColumn id="8" xr3:uid="{D548D9A8-FE15-481F-BAC8-E7E1A689769D}" name="Singapore time _x000a_(UTC+8)" dataDxfId="115" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4251,10 +4348,10 @@
     <tableColumn id="2" xr3:uid="{B7245837-75B6-40F6-AE7D-D3147CBB4F87}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{0227EB22-FBA5-4E00-B420-6E3AA6812851}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{5945C855-578A-4D8D-944D-C61D3FB10AE3}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{A1254AFE-F15E-44F5-970B-A69AE37BB049}" name="Oksana" dataDxfId="111"/>
-    <tableColumn id="4" xr3:uid="{3DBDA2FB-1ACD-4847-BD1F-DED3A5311D2A}" name="Yash" dataDxfId="110" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{C27AE526-2FCF-4366-ADC8-A03CA42351A2}" name="Shin" dataDxfId="109"/>
-    <tableColumn id="8" xr3:uid="{3AD44161-07BC-4F4F-8850-513526468727}" name="Singapore time _x000a_(UTC+8)" dataDxfId="108" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{A1254AFE-F15E-44F5-970B-A69AE37BB049}" name="Oksana" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{3DBDA2FB-1ACD-4847-BD1F-DED3A5311D2A}" name="Yash" dataDxfId="113" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{C27AE526-2FCF-4366-ADC8-A03CA42351A2}" name="Shin" dataDxfId="112"/>
+    <tableColumn id="8" xr3:uid="{3AD44161-07BC-4F4F-8850-513526468727}" name="Singapore time _x000a_(UTC+8)" dataDxfId="111" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4273,10 +4370,10 @@
     <tableColumn id="2" xr3:uid="{F9476C72-12A2-4616-8745-CE1978BCDE37}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{605B05E6-A0A4-4C17-996F-2C24B0A0EDF1}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{5E3CCE41-1A68-47E6-9FCC-C605E201F2D8}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{C4C29526-C137-4E18-B95A-6753FE3D47B6}" name="Oksana" dataDxfId="107"/>
-    <tableColumn id="4" xr3:uid="{4F2132BE-0CFB-451C-9EC1-E1506E6918A5}" name="Yash" dataDxfId="106" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{0FAD427F-9DA9-48B5-8567-DAC6D21995E5}" name="Shin" dataDxfId="105"/>
-    <tableColumn id="8" xr3:uid="{4456E27B-B965-460D-9037-A4D3B8DCF119}" name="Singapore time _x000a_(UTC+8)" dataDxfId="104" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{C4C29526-C137-4E18-B95A-6753FE3D47B6}" name="Oksana" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{4F2132BE-0CFB-451C-9EC1-E1506E6918A5}" name="Yash" dataDxfId="109" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{0FAD427F-9DA9-48B5-8567-DAC6D21995E5}" name="Shin" dataDxfId="108"/>
+    <tableColumn id="8" xr3:uid="{4456E27B-B965-460D-9037-A4D3B8DCF119}" name="Singapore time _x000a_(UTC+8)" dataDxfId="107" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4295,10 +4392,10 @@
     <tableColumn id="2" xr3:uid="{510FAB12-05D2-477C-A3C3-F37BC0D1851C}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{84C89E58-AF96-4486-932D-9F1C4010D50B}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{47B8EDD7-F35D-4B15-9091-5425488CF46B}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{F601B36D-7341-43F2-B007-B083A9D0329C}" name="Oksana" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{4D49D71A-C32F-4F3F-8515-BA31AEF1394C}" name="Yash" dataDxfId="102" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{E013925A-04D8-46D2-BE99-29E01AD91823}" name="Shin" dataDxfId="101"/>
-    <tableColumn id="8" xr3:uid="{DF2927E0-7C17-4982-BE5A-2678659A22F3}" name="Singapore time _x000a_(UTC+8)" dataDxfId="100" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{F601B36D-7341-43F2-B007-B083A9D0329C}" name="Oksana" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{4D49D71A-C32F-4F3F-8515-BA31AEF1394C}" name="Yash" dataDxfId="105" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{E013925A-04D8-46D2-BE99-29E01AD91823}" name="Shin" dataDxfId="104"/>
+    <tableColumn id="8" xr3:uid="{DF2927E0-7C17-4982-BE5A-2678659A22F3}" name="Singapore time _x000a_(UTC+8)" dataDxfId="103" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4317,10 +4414,10 @@
     <tableColumn id="2" xr3:uid="{464B2BCB-9679-42C2-9103-E4610117969B}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{A8C2F686-2137-4906-8BFB-848AE2307D9C}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{806D0D0D-AC1F-462A-9F4B-94E4E1DD514B}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{A993B93A-4341-42BF-9918-AD32E8382EA2}" name="Oksana" dataDxfId="99"/>
-    <tableColumn id="4" xr3:uid="{0E4E00EC-A3D2-4412-8607-4219225E982F}" name="Yash" dataDxfId="98" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{DA298704-D4AD-445F-8647-B6D82D739125}" name="Shin" dataDxfId="97"/>
-    <tableColumn id="8" xr3:uid="{6A2F49DA-4B3D-4DCC-9ED2-AA1F33D967E1}" name="Singapore time _x000a_(UTC+8)" dataDxfId="96" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{A993B93A-4341-42BF-9918-AD32E8382EA2}" name="Oksana" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{0E4E00EC-A3D2-4412-8607-4219225E982F}" name="Yash" dataDxfId="101" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{DA298704-D4AD-445F-8647-B6D82D739125}" name="Shin" dataDxfId="100"/>
+    <tableColumn id="8" xr3:uid="{6A2F49DA-4B3D-4DCC-9ED2-AA1F33D967E1}" name="Singapore time _x000a_(UTC+8)" dataDxfId="99" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4339,10 +4436,10 @@
     <tableColumn id="2" xr3:uid="{E62278F0-D422-41EB-9CB6-100D78481378}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{CAAFC571-90B0-4B0A-8425-47421A7E9F6D}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{5E87BB05-1B47-411C-ADEA-06B419597655}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{0CE0193C-A28C-4558-A6A7-97F61603E3D2}" name="Oksana" dataDxfId="95"/>
-    <tableColumn id="4" xr3:uid="{47608488-1168-4893-9FF9-847FEFA029E1}" name="Yash" dataDxfId="94" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{89DBE63A-BD01-43C8-8BD2-EBEA0E9D01FF}" name="Shin" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{20AC23B9-1AB5-4F2B-A645-9929067A416C}" name="Singapore time _x000a_(UTC+8)" dataDxfId="92" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{0CE0193C-A28C-4558-A6A7-97F61603E3D2}" name="Oksana" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{47608488-1168-4893-9FF9-847FEFA029E1}" name="Yash" dataDxfId="97" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{89DBE63A-BD01-43C8-8BD2-EBEA0E9D01FF}" name="Shin" dataDxfId="96"/>
+    <tableColumn id="8" xr3:uid="{20AC23B9-1AB5-4F2B-A645-9929067A416C}" name="Singapore time _x000a_(UTC+8)" dataDxfId="95" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4361,10 +4458,10 @@
     <tableColumn id="2" xr3:uid="{C41E7B5D-7252-48C5-92AE-F4C9A5741939}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{5C1CF51E-ECB1-43F0-8611-C38DD733FD23}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{6A604927-2DD8-4470-94BF-226096022555}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{CE0BB656-2D23-4E40-B245-7A1AE8DA1632}" name="Oksana" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{499C007B-9FA5-48E9-A6D5-944362D7B91E}" name="Yash" dataDxfId="90" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{E7E773A3-740E-4A98-9F17-4842D6E68C4C}" name="Shin" dataDxfId="89"/>
-    <tableColumn id="8" xr3:uid="{108A5692-38FA-4F33-B18F-274CA90DE133}" name="Singapore time _x000a_(UTC+8)" dataDxfId="88" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{CE0BB656-2D23-4E40-B245-7A1AE8DA1632}" name="Oksana" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{499C007B-9FA5-48E9-A6D5-944362D7B91E}" name="Yash" dataDxfId="93" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{E7E773A3-740E-4A98-9F17-4842D6E68C4C}" name="Shin" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{108A5692-38FA-4F33-B18F-274CA90DE133}" name="Singapore time _x000a_(UTC+8)" dataDxfId="91" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4383,10 +4480,10 @@
     <tableColumn id="2" xr3:uid="{A11049C4-7018-4D8E-BC51-A794BBEAEEE1}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{9A185BA7-BAEE-4A54-B676-09149B4DC0EC}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{5E2A4213-5435-4F61-AD75-83035A00BD7D}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{14E9FC16-87B1-4424-8FAE-2A8DD9D6FBDE}" name="Oksana" dataDxfId="87"/>
-    <tableColumn id="4" xr3:uid="{4A2ED4EB-19D6-4E1A-BCB1-8B8397946FB4}" name="Yash" dataDxfId="86" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{25796ACD-B417-4E4C-9718-41BFF812AA95}" name="Shin" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{02B95CB9-1BBF-4310-9F74-06FE84DA5A57}" name="Singapore time _x000a_(UTC+8)" dataDxfId="84" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{14E9FC16-87B1-4424-8FAE-2A8DD9D6FBDE}" name="Oksana" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{4A2ED4EB-19D6-4E1A-BCB1-8B8397946FB4}" name="Yash" dataDxfId="89" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{25796ACD-B417-4E4C-9718-41BFF812AA95}" name="Shin" dataDxfId="88"/>
+    <tableColumn id="8" xr3:uid="{02B95CB9-1BBF-4310-9F74-06FE84DA5A57}" name="Singapore time _x000a_(UTC+8)" dataDxfId="87" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4405,10 +4502,10 @@
     <tableColumn id="2" xr3:uid="{C94180EE-1407-4985-8FC4-31B24FD20334}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{C6273117-9D1B-4E78-A8BD-B9AFC0FEA4E0}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{28390446-140E-4C34-B6AE-CB73B4D47E90}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{FD0B3E24-96C6-47B4-A820-98020DBBFAC7}" name="Oksana" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{83E5024B-18C2-4A58-86BF-B200FFC47B78}" name="Yash" dataDxfId="82" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{A8ED67B9-0069-4A4F-8052-ED45553EB363}" name="Shin" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{EAB26DA3-5EE8-4111-B78D-21F5E77834DB}" name="Singapore time _x000a_(UTC+8)" dataDxfId="80" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{FD0B3E24-96C6-47B4-A820-98020DBBFAC7}" name="Oksana" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{83E5024B-18C2-4A58-86BF-B200FFC47B78}" name="Yash" dataDxfId="85" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{A8ED67B9-0069-4A4F-8052-ED45553EB363}" name="Shin" dataDxfId="84"/>
+    <tableColumn id="8" xr3:uid="{EAB26DA3-5EE8-4111-B78D-21F5E77834DB}" name="Singapore time _x000a_(UTC+8)" dataDxfId="83" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4427,10 +4524,10 @@
     <tableColumn id="2" xr3:uid="{DF5403CA-E344-4631-B2FA-F0E9C07A0B3B}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{0EB7220C-7400-44F1-9799-008E8292B142}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{55720B1D-3AF4-4697-ABB8-12D14E619F50}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{619A8323-E827-45C2-8BBB-2DAB2D84B741}" name="Oksana" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{40089D03-ABBB-455D-8A9C-76669438AF35}" name="Yash" dataDxfId="78" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{CB8A3181-E2AD-4973-B632-C290C4479585}" name="Shin" dataDxfId="77"/>
-    <tableColumn id="8" xr3:uid="{5C7E95F3-0CD5-4B70-979F-B8A1F6972DE0}" name="Singapore time _x000a_(UTC+8)" dataDxfId="76" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{619A8323-E827-45C2-8BBB-2DAB2D84B741}" name="Oksana" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{40089D03-ABBB-455D-8A9C-76669438AF35}" name="Yash" dataDxfId="81" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{CB8A3181-E2AD-4973-B632-C290C4479585}" name="Shin" dataDxfId="80"/>
+    <tableColumn id="8" xr3:uid="{5C7E95F3-0CD5-4B70-979F-B8A1F6972DE0}" name="Singapore time _x000a_(UTC+8)" dataDxfId="79" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4449,10 +4546,10 @@
     <tableColumn id="2" xr3:uid="{3CED8CBC-F4AC-49B2-9A54-297054A0F480}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{C7966841-5D56-4560-B855-DB423787778D}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{16892C88-044A-4B79-9E9B-AA99ECEA9839}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{4AC31AC3-11DD-4459-B8E3-0380683F4CDD}" name="Oksana" dataDxfId="147"/>
-    <tableColumn id="4" xr3:uid="{E30A469A-C8B5-4182-84F5-622E27AB688A}" name="Yash" dataDxfId="146" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{D4CE159E-DDA2-4C33-94DC-D058D61EF160}" name="Shin" dataDxfId="145"/>
-    <tableColumn id="8" xr3:uid="{B85528E1-B988-4A02-BE0E-E3B35841EEED}" name="Singapore time _x000a_(UTC+8)" dataDxfId="144" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{4AC31AC3-11DD-4459-B8E3-0380683F4CDD}" name="Oksana" dataDxfId="150"/>
+    <tableColumn id="4" xr3:uid="{E30A469A-C8B5-4182-84F5-622E27AB688A}" name="Yash" dataDxfId="149" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{D4CE159E-DDA2-4C33-94DC-D058D61EF160}" name="Shin" dataDxfId="148"/>
+    <tableColumn id="8" xr3:uid="{B85528E1-B988-4A02-BE0E-E3B35841EEED}" name="Singapore time _x000a_(UTC+8)" dataDxfId="147" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4471,10 +4568,10 @@
     <tableColumn id="2" xr3:uid="{82E27544-CFE2-4FCB-929E-F38F8E8BCF72}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{BFD43BAD-D695-4D65-8BF4-7FE074F6FAC6}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{386AB347-591A-4CC2-BE5A-89A3C4CE8B1D}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{E6DDB61B-6B43-4504-A1C5-DA6B43C1D082}" name="Oksana" dataDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{9FD46C37-9846-49E5-A4C7-2A1813746D11}" name="Yash" dataDxfId="74" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{3B39D51D-17AB-4B8A-89C0-ED0B5445547E}" name="Shin" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{501A922D-1D2C-40B3-86FE-C23504129690}" name="Singapore time _x000a_(UTC+8)" dataDxfId="72" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{E6DDB61B-6B43-4504-A1C5-DA6B43C1D082}" name="Oksana" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{9FD46C37-9846-49E5-A4C7-2A1813746D11}" name="Yash" dataDxfId="77" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{3B39D51D-17AB-4B8A-89C0-ED0B5445547E}" name="Shin" dataDxfId="76"/>
+    <tableColumn id="8" xr3:uid="{501A922D-1D2C-40B3-86FE-C23504129690}" name="Singapore time _x000a_(UTC+8)" dataDxfId="75" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4493,10 +4590,10 @@
     <tableColumn id="2" xr3:uid="{10F2AFDE-A8B8-4625-BAA7-CB80BAB19A74}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{7DECF3E4-30A3-41C2-9278-3705B2CF40DB}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{A5C5B894-258A-4E94-BB90-F0A974DB7A6C}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{B81A327C-68A3-4773-BCB7-505D23236337}" name="Oksana" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{05CDC919-66B1-4DCB-9E59-D282BFF82DFD}" name="Yash" dataDxfId="70" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{2BF937E2-1A8F-4DBC-AE66-C7B9F04F6957}" name="Shin" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{7967EBDF-91AA-4661-BD61-A04BE29D5B1A}" name="Singapore time _x000a_(UTC+8)" dataDxfId="68" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{B81A327C-68A3-4773-BCB7-505D23236337}" name="Oksana" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{05CDC919-66B1-4DCB-9E59-D282BFF82DFD}" name="Yash" dataDxfId="73" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{2BF937E2-1A8F-4DBC-AE66-C7B9F04F6957}" name="Shin" dataDxfId="72"/>
+    <tableColumn id="8" xr3:uid="{7967EBDF-91AA-4661-BD61-A04BE29D5B1A}" name="Singapore time _x000a_(UTC+8)" dataDxfId="71" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4515,10 +4612,10 @@
     <tableColumn id="2" xr3:uid="{CE59DEA0-9236-4D4E-BE63-600CB1F2627F}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{DF15F544-5901-4042-ACFC-62AA35048C59}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{AA60B96D-C403-41BC-8BF3-726171B925D7}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{8083B1D9-9EDE-4795-B8A5-F395FBE27404}" name="Oksana" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{9D8165AB-2615-4455-8332-2335EFC1A04C}" name="Yash" dataDxfId="66" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{76C34ED5-F333-44D4-A7B9-F005365DE0CE}" name="Shin" dataDxfId="65"/>
-    <tableColumn id="8" xr3:uid="{24C9FD46-13BE-4710-9948-40B8717FF3D7}" name="Singapore time _x000a_(UTC+8)" dataDxfId="64" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{8083B1D9-9EDE-4795-B8A5-F395FBE27404}" name="Oksana" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{9D8165AB-2615-4455-8332-2335EFC1A04C}" name="Yash" dataDxfId="69" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{76C34ED5-F333-44D4-A7B9-F005365DE0CE}" name="Shin" dataDxfId="68"/>
+    <tableColumn id="8" xr3:uid="{24C9FD46-13BE-4710-9948-40B8717FF3D7}" name="Singapore time _x000a_(UTC+8)" dataDxfId="67" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4537,10 +4634,10 @@
     <tableColumn id="2" xr3:uid="{F7A4435C-F5DA-43E5-96E8-2666A7DE6C5D}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{24037A76-A296-4FCD-B87D-C98A1655B019}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{DA68FFB9-CDF9-4FA8-9E7F-AC89FD09986A}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{0E104BBD-58A0-4A88-8980-00CBDB96C899}" name="Oksana" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{D9A092F1-2821-4B0D-BD9B-DB93139DD4A0}" name="Yash" dataDxfId="62" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{799D8249-8B89-4BFF-8AE3-BB05393B0F0E}" name="Shin" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{0A5E0F8B-DAFF-410A-A6E8-9CF9E04C85F8}" name="Singapore time _x000a_(UTC+8)" dataDxfId="60" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{0E104BBD-58A0-4A88-8980-00CBDB96C899}" name="Oksana" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{D9A092F1-2821-4B0D-BD9B-DB93139DD4A0}" name="Yash" dataDxfId="65" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{799D8249-8B89-4BFF-8AE3-BB05393B0F0E}" name="Shin" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{0A5E0F8B-DAFF-410A-A6E8-9CF9E04C85F8}" name="Singapore time _x000a_(UTC+8)" dataDxfId="63" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4559,10 +4656,10 @@
     <tableColumn id="2" xr3:uid="{2B89BE19-628C-43B9-9A4F-FD8692426C08}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{247E3465-550A-4E14-84D4-EA3481167E5A}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{01C84747-0BDD-4DEF-AC61-87B11910F555}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{63A0F4AF-ACE9-4A7E-AA1D-E34EC58D7679}" name="Oksana" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{FC1C9F78-1715-44A7-B437-8B393BC9B7D3}" name="Yash" dataDxfId="58" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{2B97574E-727C-47AB-9679-1A526BF57566}" name="Shin" dataDxfId="57"/>
-    <tableColumn id="8" xr3:uid="{5339B706-4BF0-4D38-9C15-B0A8B2D88B13}" name="Singapore time _x000a_(UTC+8)" dataDxfId="56" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{63A0F4AF-ACE9-4A7E-AA1D-E34EC58D7679}" name="Oksana" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{FC1C9F78-1715-44A7-B437-8B393BC9B7D3}" name="Yash" dataDxfId="61" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{2B97574E-727C-47AB-9679-1A526BF57566}" name="Shin" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{5339B706-4BF0-4D38-9C15-B0A8B2D88B13}" name="Singapore time _x000a_(UTC+8)" dataDxfId="59" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4581,10 +4678,10 @@
     <tableColumn id="2" xr3:uid="{7827D7BB-C78D-453E-A7F5-5EDDDECC7B77}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{34C52336-5EB3-4B4A-962F-0ABEECC6F20B}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{385B235D-CDDC-4630-A31C-93CE09396031}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{30828DC7-BDD1-4CFE-B4F0-D1D92018E809}" name="Oksana" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{1A42C202-FF37-4F9F-A497-1036B9FF987A}" name="Yash" dataDxfId="54" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{CA61A775-4A1F-46BF-B978-84391BC86856}" name="Shin" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{945CC8DC-9DF2-469C-9476-132642485561}" name="Singapore time _x000a_(UTC+8)" dataDxfId="52" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{30828DC7-BDD1-4CFE-B4F0-D1D92018E809}" name="Oksana" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{1A42C202-FF37-4F9F-A497-1036B9FF987A}" name="Yash" dataDxfId="57" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{CA61A775-4A1F-46BF-B978-84391BC86856}" name="Shin" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{945CC8DC-9DF2-469C-9476-132642485561}" name="Singapore time _x000a_(UTC+8)" dataDxfId="55" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4603,10 +4700,10 @@
     <tableColumn id="2" xr3:uid="{CF15D9C0-1B5E-4D51-8CFD-9C9811ADAAB3}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{D775262F-5CAC-4E3B-B2A9-A86E78D2B760}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{77BECF23-AAE1-4FDE-B07B-1B5A963BF75D}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{B7D3DFDA-4EDC-4D44-9EF4-1D6976EA519C}" name="Oksana" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{6F23ECFE-BE6C-4222-8DCB-BD7C28236252}" name="Yash" dataDxfId="50" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{798A1FB7-892F-4CD7-B1E0-CFB789B7ADE7}" name="Shin" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{5B8E069F-A14B-4129-A3DA-182C7B74AB91}" name="Singapore time _x000a_(UTC+8)" dataDxfId="48" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{B7D3DFDA-4EDC-4D44-9EF4-1D6976EA519C}" name="Oksana" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{6F23ECFE-BE6C-4222-8DCB-BD7C28236252}" name="Yash" dataDxfId="53" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{798A1FB7-892F-4CD7-B1E0-CFB789B7ADE7}" name="Shin" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{5B8E069F-A14B-4129-A3DA-182C7B74AB91}" name="Singapore time _x000a_(UTC+8)" dataDxfId="51" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4625,10 +4722,10 @@
     <tableColumn id="2" xr3:uid="{49FE5D61-7D29-4313-898A-830774DBD47A}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{90EA046A-3464-4813-A515-441DB628E5D4}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{6F68C3E9-22B1-412D-8561-CDB82609A974}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{997243AE-D74A-468F-BC45-E976BEF8E58D}" name="Oksana" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{E20EBAD6-A4C1-423C-9283-4E0C3BDA1350}" name="Yash" dataDxfId="46" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{966F6989-E79C-4EB4-B552-1CC87CF07D43}" name="Shin" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{181BB4EE-E469-4446-B202-B7A4812E9037}" name="Singapore time _x000a_(UTC+8)" dataDxfId="44" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{997243AE-D74A-468F-BC45-E976BEF8E58D}" name="Oksana" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{E20EBAD6-A4C1-423C-9283-4E0C3BDA1350}" name="Yash" dataDxfId="49" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{966F6989-E79C-4EB4-B552-1CC87CF07D43}" name="Shin" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{181BB4EE-E469-4446-B202-B7A4812E9037}" name="Singapore time _x000a_(UTC+8)" dataDxfId="47" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4647,10 +4744,10 @@
     <tableColumn id="2" xr3:uid="{03308F6F-7210-41F4-9A07-5979E98F17A9}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{A6C76DF6-FD7A-4B5B-882F-1CB21320DF76}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{56992E42-B37C-4386-ADAA-6BFDC7965FFE}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{5BA72103-0DCF-431E-BCDD-9671DC826774}" name="Oksana" dataDxfId="43"/>
-    <tableColumn id="4" xr3:uid="{021FBF7B-FB9D-418B-BABE-9F92D500EBC1}" name="Yash" dataDxfId="42" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{31928D4D-A400-43CB-A70B-9F9DABB5CC2F}" name="Shin" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{9CB24077-D37D-4C75-8756-CC9A92113D24}" name="Singapore time _x000a_(UTC+8)" dataDxfId="40" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{5BA72103-0DCF-431E-BCDD-9671DC826774}" name="Oksana" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{021FBF7B-FB9D-418B-BABE-9F92D500EBC1}" name="Yash" dataDxfId="45" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{31928D4D-A400-43CB-A70B-9F9DABB5CC2F}" name="Shin" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{9CB24077-D37D-4C75-8756-CC9A92113D24}" name="Singapore time _x000a_(UTC+8)" dataDxfId="43" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4669,10 +4766,10 @@
     <tableColumn id="2" xr3:uid="{31480843-9B73-4338-93C3-7BD9399442EA}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{A90BA791-6066-47FD-9350-3E02120E2D64}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{C66952DF-A7AB-4652-9624-12AD4334047E}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{3FC00AFD-60E2-415C-A416-108DAAE42808}" name="Oksana" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{0D4E04DE-C8CC-43D7-A815-179E184D113B}" name="Yash" dataDxfId="38" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{E51FD00D-B5CE-4D91-861D-48A1B0745A3C}" name="Shin" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{8F6CE992-6306-4E87-A620-8A02203F8239}" name="Singapore time _x000a_(UTC+8)" dataDxfId="36" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{3FC00AFD-60E2-415C-A416-108DAAE42808}" name="Oksana" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{0D4E04DE-C8CC-43D7-A815-179E184D113B}" name="Yash" dataDxfId="41" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{E51FD00D-B5CE-4D91-861D-48A1B0745A3C}" name="Shin" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{8F6CE992-6306-4E87-A620-8A02203F8239}" name="Singapore time _x000a_(UTC+8)" dataDxfId="39" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4691,10 +4788,10 @@
     <tableColumn id="2" xr3:uid="{4C022EB9-B856-46FA-8BCB-4AAFADB436D0}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{DB5C6103-1EB3-4D87-BCCD-B1449ACB0627}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{958629D4-4202-4E10-A49C-029FA13BC2B5}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{2E82CE34-D49B-43F6-A410-04D08B4D4A6D}" name="Oksana" dataDxfId="143"/>
-    <tableColumn id="4" xr3:uid="{A5222911-A295-4CB4-B323-FEAF8437E8BE}" name="Yash" dataDxfId="142" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{DD866F41-4DA9-430E-90BA-EE9D619A80A0}" name="Shin" dataDxfId="141"/>
-    <tableColumn id="8" xr3:uid="{62BE29B6-6643-43DA-A5D7-7DA544D19372}" name="Singapore time _x000a_(UTC+8)" dataDxfId="140" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{2E82CE34-D49B-43F6-A410-04D08B4D4A6D}" name="Oksana" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{A5222911-A295-4CB4-B323-FEAF8437E8BE}" name="Yash" dataDxfId="145" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{DD866F41-4DA9-430E-90BA-EE9D619A80A0}" name="Shin" dataDxfId="144"/>
+    <tableColumn id="8" xr3:uid="{62BE29B6-6643-43DA-A5D7-7DA544D19372}" name="Singapore time _x000a_(UTC+8)" dataDxfId="143" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4713,10 +4810,10 @@
     <tableColumn id="2" xr3:uid="{54FD0529-ADCD-4B53-B89F-E86041948760}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{90F149A0-726C-46FC-84B2-9F8DEBCD7A8A}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{A4E2FD44-3916-4E9E-8FA7-0FFE817BC883}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{06A7359E-3492-4A46-A918-245234F01777}" name="Oksana" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{E7837638-3B4F-4E05-8AB9-D3E2A4CEE16D}" name="Yash" dataDxfId="34" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{A02E9D25-A3F7-419D-B22E-AB47BDDA1820}" name="Shin" dataDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{A2D2FFF8-7AE7-4A5A-B8F4-0BB9750B3F80}" name="Singapore time _x000a_(UTC+8)" dataDxfId="32" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{06A7359E-3492-4A46-A918-245234F01777}" name="Oksana" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{E7837638-3B4F-4E05-8AB9-D3E2A4CEE16D}" name="Yash" dataDxfId="37" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{A02E9D25-A3F7-419D-B22E-AB47BDDA1820}" name="Shin" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{A2D2FFF8-7AE7-4A5A-B8F4-0BB9750B3F80}" name="Singapore time _x000a_(UTC+8)" dataDxfId="35" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4735,10 +4832,10 @@
     <tableColumn id="2" xr3:uid="{EEA6CB8E-095C-4E58-9685-A72D229B6858}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{6DC39266-36A3-4946-8DCE-8B47BB9B4183}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{A76FAE03-CD47-4F58-BAAA-E0B399383AAF}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{D1745B88-2A19-4C36-8376-5D7554546772}" name="Oksana" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{B606433D-ED39-4EA8-B1F3-D99C37D328F4}" name="Yash" dataDxfId="30" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{9F53371F-710F-47AE-B351-1E775BE55F61}" name="Shin" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{ADD98C06-1826-4DE0-AEA5-DB7B683D012A}" name="Singapore time _x000a_(UTC+8)" dataDxfId="28" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{D1745B88-2A19-4C36-8376-5D7554546772}" name="Oksana" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{B606433D-ED39-4EA8-B1F3-D99C37D328F4}" name="Yash" dataDxfId="33" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{9F53371F-710F-47AE-B351-1E775BE55F61}" name="Shin" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{ADD98C06-1826-4DE0-AEA5-DB7B683D012A}" name="Singapore time _x000a_(UTC+8)" dataDxfId="31" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4757,10 +4854,10 @@
     <tableColumn id="2" xr3:uid="{C0E329BF-1DCB-4D86-A33C-365B440B70E7}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{003F982F-BD88-4265-93AF-64094B13BDFB}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{F89F2619-1757-4DDE-AFC6-B7187DA84CBB}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{AAC4B066-8416-45EE-B03C-810F350FD500}" name="Oksana" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{99851EA6-3B00-42BA-BA64-2C6BADB94400}" name="Yash" dataDxfId="26" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{443DF852-C91E-4BAF-A7AF-30CA8C46D5C1}" name="Shin" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{66E96285-11C2-4BC0-B1C5-37FE887C6CA0}" name="Singapore time _x000a_(UTC+8)" dataDxfId="24" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{AAC4B066-8416-45EE-B03C-810F350FD500}" name="Oksana" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{99851EA6-3B00-42BA-BA64-2C6BADB94400}" name="Yash" dataDxfId="29" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{443DF852-C91E-4BAF-A7AF-30CA8C46D5C1}" name="Shin" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{66E96285-11C2-4BC0-B1C5-37FE887C6CA0}" name="Singapore time _x000a_(UTC+8)" dataDxfId="27" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4779,10 +4876,10 @@
     <tableColumn id="2" xr3:uid="{64619660-65D6-4C45-BC25-67A7E10F3358}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{EE17890D-92A4-4A8E-AF68-AD5B0E4DE02A}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{B0DCC0DC-F3ED-48D9-8EBD-678B062883D7}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{4E5BC969-05EA-45B7-BEED-39380C81156B}" name="Oksana" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{E996A125-351B-4D4B-B633-729E72E94692}" name="Yash" dataDxfId="22" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{09825810-304A-4FB8-854B-0DF218A934B4}" name="Shin" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{29ADBCC6-6218-4EE5-A99E-0A7C46223547}" name="Singapore time _x000a_(UTC+8)" dataDxfId="20" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{4E5BC969-05EA-45B7-BEED-39380C81156B}" name="Oksana" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{E996A125-351B-4D4B-B633-729E72E94692}" name="Yash" dataDxfId="25" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{09825810-304A-4FB8-854B-0DF218A934B4}" name="Shin" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{29ADBCC6-6218-4EE5-A99E-0A7C46223547}" name="Singapore time _x000a_(UTC+8)" dataDxfId="23" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4801,10 +4898,10 @@
     <tableColumn id="2" xr3:uid="{443189F4-32D8-468C-9055-BDC7AD9CD990}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{EBCEC7EE-23ED-4FAF-8B83-46D11C025580}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{E3B2AFF1-955C-47F4-B38F-D11790DB9CB7}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{D83852B9-BEDE-41D1-A364-1CBB8FD746D0}" name="Oksana" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{714DE460-DD0B-472B-B461-8DC5E402A1A7}" name="Yash" dataDxfId="18" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{B14AD5A6-80B6-437A-AE2B-23C39AA1D815}" name="Shin" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{FFE787F0-213E-4544-99EB-6744043A39EF}" name="Singapore time _x000a_(UTC+8)" dataDxfId="16" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{D83852B9-BEDE-41D1-A364-1CBB8FD746D0}" name="Oksana" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{714DE460-DD0B-472B-B461-8DC5E402A1A7}" name="Yash" dataDxfId="21" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{B14AD5A6-80B6-437A-AE2B-23C39AA1D815}" name="Shin" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{FFE787F0-213E-4544-99EB-6744043A39EF}" name="Singapore time _x000a_(UTC+8)" dataDxfId="19" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4823,10 +4920,10 @@
     <tableColumn id="2" xr3:uid="{4D3D2ADB-B410-4BB3-92F0-5796EF387FD6}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{BBB04EDB-D05B-42A2-BA84-AB8CFFF17C8C}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{0B6B181D-59AF-48AE-B2F7-9B8848D9B577}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{2EBD93C7-4EE1-43BA-A143-49BA390F2A4D}" name="Oksana" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{E9EEED46-6A74-4194-9603-D11216CEA4C8}" name="Yash" dataDxfId="14" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{3E3816D0-F57B-4BAA-8AB3-7E9236C67E78}" name="Shin" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{1FD3A54C-3F10-42D9-8255-0E9C2E4E3E5D}" name="Singapore time _x000a_(UTC+8)" dataDxfId="12" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{2EBD93C7-4EE1-43BA-A143-49BA390F2A4D}" name="Oksana" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{E9EEED46-6A74-4194-9603-D11216CEA4C8}" name="Yash" dataDxfId="17" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{3E3816D0-F57B-4BAA-8AB3-7E9236C67E78}" name="Shin" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{1FD3A54C-3F10-42D9-8255-0E9C2E4E3E5D}" name="Singapore time _x000a_(UTC+8)" dataDxfId="15" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4845,10 +4942,10 @@
     <tableColumn id="2" xr3:uid="{CD5272FA-F49A-4BE8-948F-8EF3E3E7AE75}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{ECD03D01-EDB4-47B6-B1C9-690C5BC6DBEA}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{4AA58E18-12DB-4F38-8402-929EE81E6FBD}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{8ADC5D84-1E94-4A8E-A0E4-CFA2F146D0E0}" name="Oksana" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{368999B6-116C-45B1-BE5E-2FD396AB7CD3}" name="Yash" dataDxfId="10" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{4EDC2545-0024-49C6-995B-A3D7551C9993}" name="Shin" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{63CFD507-E60C-4990-93F5-FC7969499501}" name="Singapore time _x000a_(UTC+8)" dataDxfId="8" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{8ADC5D84-1E94-4A8E-A0E4-CFA2F146D0E0}" name="Oksana" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{368999B6-116C-45B1-BE5E-2FD396AB7CD3}" name="Yash" dataDxfId="13" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{4EDC2545-0024-49C6-995B-A3D7551C9993}" name="Shin" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{63CFD507-E60C-4990-93F5-FC7969499501}" name="Singapore time _x000a_(UTC+8)" dataDxfId="11" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4867,10 +4964,10 @@
     <tableColumn id="2" xr3:uid="{A2088134-3A7C-4DE9-B0F3-AA7574753BDE}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{9521E4C5-7D16-40BD-8736-5774F4A03DE5}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{C16241CE-FCD4-4B92-8C75-1E60871988FC}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{296FFE1F-244D-40AD-9291-90D8E9BABD74}" name="Oksana" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{F37EF47C-EF59-4BB4-A588-29A733234107}" name="Yash" dataDxfId="6" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{47AF080C-B200-418C-A6A1-DE7112B3A6DB}" name="Shin" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{4F617619-63D0-41E6-806E-7FCB193CCCB0}" name="Singapore time _x000a_(UTC+8)" dataDxfId="4" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{296FFE1F-244D-40AD-9291-90D8E9BABD74}" name="Oksana" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F37EF47C-EF59-4BB4-A588-29A733234107}" name="Yash" dataDxfId="9" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{47AF080C-B200-418C-A6A1-DE7112B3A6DB}" name="Shin" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{4F617619-63D0-41E6-806E-7FCB193CCCB0}" name="Singapore time _x000a_(UTC+8)" dataDxfId="7" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4889,10 +4986,10 @@
     <tableColumn id="2" xr3:uid="{6123AA27-D3FE-4F54-B9D1-CC55C3AED696}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{3319C129-20F6-4D73-B7CB-5325839EC3B4}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{BB0ADEA4-48EE-42C3-83CE-C03FE1EE6FA2}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{3E057A32-8FB7-438D-81C8-A3FE2889B2DA}" name="Oksana" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{29D199E5-C26D-4981-8C4C-2020018BFFA6}" name="Yash" dataDxfId="2" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{FEA767D2-6ECD-4223-9090-04E9534496AB}" name="Shin" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{8E9B045C-3723-42B7-B771-DEAF62D133F1}" name="Singapore time _x000a_(UTC+8)" dataDxfId="0" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{3E057A32-8FB7-438D-81C8-A3FE2889B2DA}" name="Oksana" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{29D199E5-C26D-4981-8C4C-2020018BFFA6}" name="Yash" dataDxfId="5" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{FEA767D2-6ECD-4223-9090-04E9534496AB}" name="Shin" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{8E9B045C-3723-42B7-B771-DEAF62D133F1}" name="Singapore time _x000a_(UTC+8)" dataDxfId="3" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4911,10 +5008,10 @@
     <tableColumn id="2" xr3:uid="{B3B0EC76-43B2-457F-BE1F-16BCD92A0D96}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{BA11EC77-4355-4978-BE05-46814D60DA77}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{A84BCF49-9E56-4C72-8815-8A724C6ECB76}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{607AD4AD-2437-49C7-8259-CFCAA36C68C7}" name="Oksana" dataDxfId="139"/>
-    <tableColumn id="4" xr3:uid="{78094C5E-5AAC-4AD0-A02D-C65615C6F3DB}" name="Yash" dataDxfId="138" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{106D26EF-FA57-428B-A6D5-030C928FE171}" name="Shin" dataDxfId="137"/>
-    <tableColumn id="8" xr3:uid="{B0FF0E58-6A04-47FA-A1A3-19FE4EF1B69E}" name="Singapore time _x000a_(UTC+8)" dataDxfId="136" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{607AD4AD-2437-49C7-8259-CFCAA36C68C7}" name="Oksana" dataDxfId="142"/>
+    <tableColumn id="4" xr3:uid="{78094C5E-5AAC-4AD0-A02D-C65615C6F3DB}" name="Yash" dataDxfId="141" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{106D26EF-FA57-428B-A6D5-030C928FE171}" name="Shin" dataDxfId="140"/>
+    <tableColumn id="8" xr3:uid="{B0FF0E58-6A04-47FA-A1A3-19FE4EF1B69E}" name="Singapore time _x000a_(UTC+8)" dataDxfId="139" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4933,10 +5030,10 @@
     <tableColumn id="2" xr3:uid="{F4DCFEB0-95A0-40D6-BD6B-AF2B99525AA8}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{781764E6-E4AA-495B-B236-C628D15D5461}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{AB9BB1D3-1E78-4987-BDBA-2C92F62A218E}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{E0C104D4-001A-4F55-A83A-ADCF203F1055}" name="Oksana" dataDxfId="135"/>
-    <tableColumn id="4" xr3:uid="{79809C09-32E2-4926-8909-6F58AF319FB5}" name="Yash" dataDxfId="134" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{291A8DB2-E1F0-413D-8D3A-ECAA328E3313}" name="Shin" dataDxfId="133"/>
-    <tableColumn id="8" xr3:uid="{86192AE1-B5B3-467E-A226-C43BFA134AA4}" name="Singapore time _x000a_(UTC+8)" dataDxfId="132" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{E0C104D4-001A-4F55-A83A-ADCF203F1055}" name="Oksana" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{79809C09-32E2-4926-8909-6F58AF319FB5}" name="Yash" dataDxfId="137" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{291A8DB2-E1F0-413D-8D3A-ECAA328E3313}" name="Shin" dataDxfId="136"/>
+    <tableColumn id="8" xr3:uid="{86192AE1-B5B3-467E-A226-C43BFA134AA4}" name="Singapore time _x000a_(UTC+8)" dataDxfId="135" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4953,12 +5050,12 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5AFD8CEE-156D-4ABC-B384-928CF651B6AD}" name="UK Time _x000a_(UTC)" dataCellStyle="Time"/>
     <tableColumn id="2" xr3:uid="{7C12F197-B393-41F7-BE8B-70E939BC436F}" name="Chris"/>
-    <tableColumn id="5" xr3:uid="{7268AD0F-E73D-4840-87A1-84AE9AB98952}" name="Dom" dataCellStyle="Phone"/>
+    <tableColumn id="5" xr3:uid="{7268AD0F-E73D-4840-87A1-84AE9AB98952}" name="Dom" dataDxfId="2" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{CC9C32B8-AD75-4B6B-9E0D-BD84F9B6E326}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{B407F25D-3B70-4EA2-838A-E0762855D8DC}" name="Oksana" dataDxfId="131"/>
-    <tableColumn id="4" xr3:uid="{CED30464-2526-473F-9F46-5CBC8D0325C1}" name="Yash" dataDxfId="130" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{243E3DD0-DC7C-4880-B1AB-214F1CD8CF64}" name="Shin" dataDxfId="129"/>
-    <tableColumn id="8" xr3:uid="{A7B5023C-E854-4502-8A5F-1CD0597412C3}" name="Singapore time _x000a_(UTC+8)" dataDxfId="128" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{B407F25D-3B70-4EA2-838A-E0762855D8DC}" name="Oksana" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{CED30464-2526-473F-9F46-5CBC8D0325C1}" name="Yash" dataDxfId="133" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{243E3DD0-DC7C-4880-B1AB-214F1CD8CF64}" name="Shin" dataDxfId="132"/>
+    <tableColumn id="8" xr3:uid="{A7B5023C-E854-4502-8A5F-1CD0597412C3}" name="Singapore time _x000a_(UTC+8)" dataDxfId="131" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4975,12 +5072,12 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0F5ED816-7237-48FB-89C5-529C9F9E206E}" name="UK Time _x000a_(UTC)" dataCellStyle="Time"/>
     <tableColumn id="2" xr3:uid="{7C79677E-C8AC-4F1C-967C-1C44B093572A}" name="Chris"/>
-    <tableColumn id="5" xr3:uid="{A36C43A9-6454-4BE5-AB45-B19CB31E0D37}" name="Dom" dataCellStyle="Phone"/>
+    <tableColumn id="5" xr3:uid="{A36C43A9-6454-4BE5-AB45-B19CB31E0D37}" name="Dom" dataDxfId="0" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{2AE833C0-5922-4AFD-A44F-5A7037E2E287}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{171C9E84-7179-4AC1-BEA0-3D0278AC8F40}" name="Oksana" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{D7EB1D36-7FF1-400C-B987-B289DAECEF7C}" name="Yash" dataDxfId="126" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{2D1217D5-2902-47EC-B52C-40CD7EBCDF00}" name="Shin" dataDxfId="125"/>
-    <tableColumn id="8" xr3:uid="{A2ACC072-6C71-423E-B040-38E53AB5BA33}" name="Singapore time _x000a_(UTC+8)" dataDxfId="124" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{171C9E84-7179-4AC1-BEA0-3D0278AC8F40}" name="Oksana" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{D7EB1D36-7FF1-400C-B987-B289DAECEF7C}" name="Yash" dataDxfId="129" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{2D1217D5-2902-47EC-B52C-40CD7EBCDF00}" name="Shin" dataDxfId="128"/>
+    <tableColumn id="8" xr3:uid="{A2ACC072-6C71-423E-B040-38E53AB5BA33}" name="Singapore time _x000a_(UTC+8)" dataDxfId="127" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4997,12 +5094,12 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00A12453-B640-4475-B6A2-960B89B26633}" name="UK Time _x000a_(UTC)" dataCellStyle="Time"/>
     <tableColumn id="2" xr3:uid="{5D48B011-E5EE-47BF-B5B0-BF8C8357A2A5}" name="Chris"/>
-    <tableColumn id="5" xr3:uid="{95894411-2418-4579-86A6-175EBD884D6E}" name="Dom" dataCellStyle="Phone"/>
+    <tableColumn id="5" xr3:uid="{95894411-2418-4579-86A6-175EBD884D6E}" name="Dom" dataDxfId="1" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{90E6CFA1-354F-406E-9CB8-742306D418C5}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{5F04F278-C00A-4CB5-B21C-86DECAB44F7D}" name="Oksana" dataDxfId="123"/>
-    <tableColumn id="4" xr3:uid="{7F4DB685-C7E8-4287-8440-485BB3DCC370}" name="Yash" dataDxfId="122" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{3565CB8E-322E-4086-8C5B-1E1BFB91B9B6}" name="Shin" dataDxfId="121"/>
-    <tableColumn id="8" xr3:uid="{94FB360C-7BA2-488D-9271-D76AF5BC7FD7}" name="Singapore time _x000a_(UTC+8)" dataDxfId="120" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{5F04F278-C00A-4CB5-B21C-86DECAB44F7D}" name="Oksana" dataDxfId="126"/>
+    <tableColumn id="4" xr3:uid="{7F4DB685-C7E8-4287-8440-485BB3DCC370}" name="Yash" dataDxfId="125" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{3565CB8E-322E-4086-8C5B-1E1BFB91B9B6}" name="Shin" dataDxfId="124"/>
+    <tableColumn id="8" xr3:uid="{94FB360C-7BA2-488D-9271-D76AF5BC7FD7}" name="Singapore time _x000a_(UTC+8)" dataDxfId="123" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -5021,10 +5118,10 @@
     <tableColumn id="2" xr3:uid="{5BAA5CC5-149B-4353-B284-4AD89F136006}" name="Chris"/>
     <tableColumn id="5" xr3:uid="{B675EEAE-3EE4-4916-B6A7-CBAF0A1AA217}" name="Dom" dataCellStyle="Phone"/>
     <tableColumn id="7" xr3:uid="{6F0297EA-A99C-4D0D-87D7-31E429E1395E}" name="Irina"/>
-    <tableColumn id="3" xr3:uid="{C55965D9-E79A-43D9-AEDD-0520AEDAB7CF}" name="Oksana" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{B1080426-3D4E-4EFB-8291-9AC031D3B4C7}" name="Yash" dataDxfId="118" dataCellStyle="Phone"/>
-    <tableColumn id="6" xr3:uid="{D578F166-E98B-4304-A703-861BB2124419}" name="Shin" dataDxfId="117"/>
-    <tableColumn id="8" xr3:uid="{8FE165A0-3692-4866-A3A4-3184BE58E8C1}" name="Singapore time _x000a_(UTC+8)" dataDxfId="116" dataCellStyle="Time"/>
+    <tableColumn id="3" xr3:uid="{C55965D9-E79A-43D9-AEDD-0520AEDAB7CF}" name="Oksana" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{B1080426-3D4E-4EFB-8291-9AC031D3B4C7}" name="Yash" dataDxfId="121" dataCellStyle="Phone"/>
+    <tableColumn id="6" xr3:uid="{D578F166-E98B-4304-A703-861BB2124419}" name="Shin" dataDxfId="120"/>
+    <tableColumn id="8" xr3:uid="{8FE165A0-3692-4866-A3A4-3184BE58E8C1}" name="Singapore time _x000a_(UTC+8)" dataDxfId="119" dataCellStyle="Time"/>
   </tableColumns>
   <tableStyleInfo name="Daily Appointment Calendar" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -5036,7 +5133,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5362,8 +5459,8 @@
   </sheetPr>
   <dimension ref="B1:AA17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5543,7 +5640,7 @@
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="4"/>
@@ -5553,7 +5650,7 @@
       <c r="K5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="11"/>
       <c r="O5" s="6"/>
       <c r="P5" s="4"/>
@@ -5563,7 +5660,7 @@
       <c r="T5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="4"/>
+      <c r="V5" s="17"/>
       <c r="W5" s="11"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="4"/>
@@ -5575,7 +5672,7 @@
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="4"/>
@@ -5585,7 +5682,7 @@
       <c r="K6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="4"/>
@@ -5595,7 +5692,7 @@
       <c r="T6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="4"/>
+      <c r="V6" s="17"/>
       <c r="W6" s="11"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="4"/>
@@ -5607,7 +5704,7 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="4"/>
@@ -5617,7 +5714,7 @@
       <c r="K7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
       <c r="P7" s="4"/>
@@ -5627,7 +5724,7 @@
       <c r="T7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="4"/>
+      <c r="V7" s="17"/>
       <c r="W7" s="11"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="4"/>
@@ -5639,7 +5736,7 @@
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="4"/>
@@ -5649,7 +5746,7 @@
       <c r="K8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="4"/>
@@ -5659,7 +5756,7 @@
       <c r="T8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V8" s="4"/>
+      <c r="V8" s="17"/>
       <c r="W8" s="11"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="4"/>
@@ -5671,7 +5768,7 @@
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="18"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="4"/>
@@ -5681,7 +5778,7 @@
       <c r="K9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
       <c r="P9" s="4"/>
@@ -5691,7 +5788,7 @@
       <c r="T9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="4"/>
+      <c r="V9" s="18"/>
       <c r="W9" s="11"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="4"/>
@@ -5703,7 +5800,7 @@
       <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="4"/>
@@ -5713,7 +5810,7 @@
       <c r="K10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="19"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="4"/>
@@ -5723,7 +5820,7 @@
       <c r="T10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="18"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="4"/>
@@ -5735,7 +5832,7 @@
       <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="18"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="4"/>
@@ -5745,7 +5842,7 @@
       <c r="K11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="4"/>
@@ -5755,7 +5852,7 @@
       <c r="T11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="V11" s="4"/>
+      <c r="V11" s="18"/>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="4"/>
@@ -5767,7 +5864,7 @@
       <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="6"/>
       <c r="F12" s="11"/>
       <c r="G12" s="4"/>
@@ -5777,7 +5874,7 @@
       <c r="K12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="4"/>
@@ -5787,7 +5884,7 @@
       <c r="T12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="V12" s="4"/>
+      <c r="V12" s="17"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="4"/>
@@ -5799,7 +5896,7 @@
       <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="6"/>
       <c r="F13" s="11"/>
       <c r="G13" s="4"/>
@@ -5809,7 +5906,7 @@
       <c r="K13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="17"/>
       <c r="N13" s="6"/>
       <c r="O13" s="12"/>
       <c r="P13" s="4"/>
@@ -5819,7 +5916,7 @@
       <c r="T13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="4"/>
+      <c r="V13" s="17"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="4"/>
@@ -5831,7 +5928,7 @@
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="4"/>
@@ -5841,7 +5938,7 @@
       <c r="K14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="17"/>
       <c r="N14" s="6"/>
       <c r="O14" s="12"/>
       <c r="P14" s="4"/>
@@ -5851,7 +5948,7 @@
       <c r="T14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="V14" s="4"/>
+      <c r="V14" s="17"/>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="4"/>
@@ -5863,7 +5960,7 @@
       <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="4"/>
@@ -5873,7 +5970,7 @@
       <c r="K15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="17"/>
       <c r="N15" s="6"/>
       <c r="O15" s="12"/>
       <c r="P15" s="4"/>
@@ -5883,7 +5980,7 @@
       <c r="T15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="V15" s="4"/>
+      <c r="V15" s="17"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="4"/>
@@ -5961,8 +6058,8 @@
   </sheetPr>
   <dimension ref="B1:BK17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14:N15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="AE5" sqref="AE5:AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6358,7 +6455,7 @@
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="4"/>
@@ -6368,7 +6465,7 @@
       <c r="K5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="17"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
       <c r="P5" s="4"/>
@@ -6378,7 +6475,7 @@
       <c r="T5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="4"/>
+      <c r="V5" s="18"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="4"/>
       <c r="AA5" s="5" t="s">
@@ -6387,7 +6484,7 @@
       <c r="AC5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AE5" s="4"/>
+      <c r="AE5" s="17"/>
       <c r="AG5" s="12"/>
       <c r="AH5" s="4"/>
       <c r="AJ5" s="5" t="s">
@@ -6396,7 +6493,7 @@
       <c r="AL5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AN5" s="4"/>
+      <c r="AN5" s="18"/>
       <c r="AP5" s="11"/>
       <c r="AQ5" s="4"/>
       <c r="AS5" s="5" t="s">
@@ -6425,7 +6522,7 @@
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="4"/>
@@ -6435,7 +6532,7 @@
       <c r="K6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="17"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
       <c r="P6" s="4"/>
@@ -6445,7 +6542,7 @@
       <c r="T6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="V6" s="4"/>
+      <c r="V6" s="18"/>
       <c r="X6" s="11"/>
       <c r="Y6" s="4"/>
       <c r="AA6" s="5" t="s">
@@ -6454,7 +6551,7 @@
       <c r="AC6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AE6" s="4"/>
+      <c r="AE6" s="17"/>
       <c r="AG6" s="12"/>
       <c r="AH6" s="4"/>
       <c r="AJ6" s="5" t="s">
@@ -6463,7 +6560,7 @@
       <c r="AL6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AN6" s="4"/>
+      <c r="AN6" s="18"/>
       <c r="AP6" s="11"/>
       <c r="AQ6" s="4"/>
       <c r="AS6" s="5" t="s">
@@ -6492,7 +6589,7 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="6"/>
       <c r="F7" s="12"/>
       <c r="G7" s="4"/>
@@ -6502,7 +6599,7 @@
       <c r="K7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="17"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
       <c r="P7" s="4"/>
@@ -6512,7 +6609,7 @@
       <c r="T7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="4"/>
+      <c r="V7" s="18"/>
       <c r="X7" s="11"/>
       <c r="Y7" s="4"/>
       <c r="AA7" s="5" t="s">
@@ -6521,7 +6618,7 @@
       <c r="AC7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AE7" s="4"/>
+      <c r="AE7" s="17"/>
       <c r="AG7" s="12"/>
       <c r="AH7" s="4"/>
       <c r="AJ7" s="5" t="s">
@@ -6530,7 +6627,7 @@
       <c r="AL7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AN7" s="4"/>
+      <c r="AN7" s="18"/>
       <c r="AP7" s="11"/>
       <c r="AQ7" s="4"/>
       <c r="AS7" s="5" t="s">
@@ -6559,7 +6656,7 @@
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
       <c r="G8" s="4"/>
@@ -6569,7 +6666,7 @@
       <c r="K8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="17"/>
       <c r="N8" s="12"/>
       <c r="O8" s="11"/>
       <c r="P8" s="4"/>
@@ -6579,7 +6676,7 @@
       <c r="T8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V8" s="4"/>
+      <c r="V8" s="18"/>
       <c r="X8" s="11"/>
       <c r="Y8" s="4"/>
       <c r="AA8" s="5" t="s">
@@ -6588,7 +6685,7 @@
       <c r="AC8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AE8" s="4"/>
+      <c r="AE8" s="17"/>
       <c r="AG8" s="12"/>
       <c r="AH8" s="4"/>
       <c r="AJ8" s="5" t="s">
@@ -6597,7 +6694,7 @@
       <c r="AL8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AN8" s="4"/>
+      <c r="AN8" s="18"/>
       <c r="AP8" s="11"/>
       <c r="AQ8" s="4"/>
       <c r="AS8" s="5" t="s">
@@ -6626,7 +6723,7 @@
       <c r="B9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9" s="4"/>
@@ -6636,7 +6733,7 @@
       <c r="K9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="18"/>
       <c r="N9" s="12"/>
       <c r="O9" s="11"/>
       <c r="P9" s="4"/>
@@ -6646,7 +6743,7 @@
       <c r="T9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="4"/>
+      <c r="V9" s="17"/>
       <c r="X9" s="11"/>
       <c r="Y9" s="4"/>
       <c r="AA9" s="10" t="s">
@@ -6655,7 +6752,7 @@
       <c r="AC9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AE9" s="4"/>
+      <c r="AE9" s="18"/>
       <c r="AG9" s="12"/>
       <c r="AH9" s="4"/>
       <c r="AJ9" s="10" t="s">
@@ -6664,7 +6761,7 @@
       <c r="AL9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="AN9" s="4"/>
+      <c r="AN9" s="17"/>
       <c r="AP9" s="11"/>
       <c r="AQ9" s="4"/>
       <c r="AS9" s="10" t="s">
@@ -6693,7 +6790,7 @@
       <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
       <c r="G10" s="4"/>
@@ -6703,7 +6800,7 @@
       <c r="K10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="18"/>
       <c r="N10" s="12"/>
       <c r="O10" s="11"/>
       <c r="P10" s="4"/>
@@ -6713,7 +6810,7 @@
       <c r="T10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="17"/>
       <c r="X10" s="11"/>
       <c r="Y10" s="4"/>
       <c r="AA10" s="10" t="s">
@@ -6722,7 +6819,7 @@
       <c r="AC10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AE10" s="4"/>
+      <c r="AE10" s="18"/>
       <c r="AG10" s="12"/>
       <c r="AH10" s="4"/>
       <c r="AJ10" s="10" t="s">
@@ -6731,7 +6828,7 @@
       <c r="AL10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="AN10" s="4"/>
+      <c r="AN10" s="17"/>
       <c r="AP10" s="11"/>
       <c r="AQ10" s="4"/>
       <c r="AS10" s="10" t="s">
@@ -6760,7 +6857,7 @@
       <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
       <c r="G11" s="4"/>
@@ -6770,7 +6867,7 @@
       <c r="K11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="18"/>
       <c r="N11" s="12"/>
       <c r="O11" s="11"/>
       <c r="P11" s="4"/>
@@ -6780,7 +6877,7 @@
       <c r="T11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="V11" s="4"/>
+      <c r="V11" s="16"/>
       <c r="X11" s="11"/>
       <c r="Y11" s="4"/>
       <c r="AA11" s="10" t="s">
@@ -6789,7 +6886,7 @@
       <c r="AC11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AE11" s="4"/>
+      <c r="AE11" s="18"/>
       <c r="AG11" s="12"/>
       <c r="AH11" s="4"/>
       <c r="AJ11" s="10" t="s">
@@ -6798,7 +6895,7 @@
       <c r="AL11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AN11" s="4"/>
+      <c r="AN11" s="16"/>
       <c r="AP11" s="11"/>
       <c r="AQ11" s="4"/>
       <c r="AS11" s="10" t="s">
@@ -6827,7 +6924,7 @@
       <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="18"/>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
       <c r="G12" s="4"/>
@@ -6837,7 +6934,7 @@
       <c r="K12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="18"/>
       <c r="N12" s="12"/>
       <c r="O12" s="11"/>
       <c r="P12" s="4"/>
@@ -6847,7 +6944,7 @@
       <c r="T12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="V12" s="4"/>
+      <c r="V12" s="18"/>
       <c r="X12" s="11"/>
       <c r="Y12" s="4"/>
       <c r="AA12" s="10" t="s">
@@ -6856,7 +6953,7 @@
       <c r="AC12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AE12" s="4"/>
+      <c r="AE12" s="18"/>
       <c r="AG12" s="12"/>
       <c r="AH12" s="4"/>
       <c r="AJ12" s="10" t="s">
@@ -6865,7 +6962,7 @@
       <c r="AL12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AN12" s="4"/>
+      <c r="AN12" s="18"/>
       <c r="AP12" s="11"/>
       <c r="AQ12" s="4"/>
       <c r="AS12" s="10" t="s">
@@ -6894,7 +6991,7 @@
       <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="18"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="4"/>
@@ -6904,7 +7001,7 @@
       <c r="K13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="16"/>
       <c r="N13" s="12"/>
       <c r="O13" s="11"/>
       <c r="P13" s="4"/>
@@ -6914,7 +7011,7 @@
       <c r="T13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="4"/>
+      <c r="V13" s="18"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="4"/>
       <c r="AA13" s="10" t="s">
@@ -6923,7 +7020,7 @@
       <c r="AC13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AE13" s="4"/>
+      <c r="AE13" s="16"/>
       <c r="AG13" s="12"/>
       <c r="AH13" s="4"/>
       <c r="AJ13" s="10" t="s">
@@ -6932,7 +7029,7 @@
       <c r="AL13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AN13" s="4"/>
+      <c r="AN13" s="18"/>
       <c r="AP13" s="11"/>
       <c r="AQ13" s="4"/>
       <c r="AS13" s="10" t="s">
@@ -6961,7 +7058,7 @@
       <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="4"/>
@@ -6971,7 +7068,7 @@
       <c r="K14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="4"/>
@@ -6981,7 +7078,7 @@
       <c r="T14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="V14" s="4"/>
+      <c r="V14" s="16"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="4"/>
       <c r="AA14" s="10" t="s">
@@ -6990,7 +7087,7 @@
       <c r="AC14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AE14" s="4"/>
+      <c r="AE14" s="16"/>
       <c r="AG14" s="12"/>
       <c r="AH14" s="4"/>
       <c r="AJ14" s="10" t="s">
@@ -6999,7 +7096,7 @@
       <c r="AL14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AN14" s="4"/>
+      <c r="AN14" s="16"/>
       <c r="AP14" s="12"/>
       <c r="AQ14" s="4"/>
       <c r="AS14" s="10" t="s">
@@ -7028,7 +7125,7 @@
       <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="4"/>
@@ -7038,7 +7135,7 @@
       <c r="K15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M15" s="4"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="4"/>
@@ -7048,7 +7145,7 @@
       <c r="T15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="V15" s="4"/>
+      <c r="V15" s="16"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="4"/>
       <c r="AA15" s="10" t="s">
@@ -7057,7 +7154,7 @@
       <c r="AC15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AE15" s="4"/>
+      <c r="AE15" s="16"/>
       <c r="AG15" s="12"/>
       <c r="AH15" s="4"/>
       <c r="AJ15" s="10" t="s">
@@ -7066,7 +7163,7 @@
       <c r="AL15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN15" s="4"/>
+      <c r="AN15" s="16"/>
       <c r="AP15" s="12"/>
       <c r="AQ15" s="4"/>
       <c r="AS15" s="10" t="s">
@@ -7153,12 +7250,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="T3:U3"/>
     <mergeCell ref="BD3:BE3"/>
     <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="AC3:AD3"/>
@@ -7167,6 +7258,12 @@
     <mergeCell ref="AO3:AQ3"/>
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="E4 H4 N4 Q4 W4 Z4 AF4 AI4 AO4 AR4 AX4 BA4 BG4 BJ4" xr:uid="{277197B0-7949-4A5D-BABB-94B0331D06DB}"/>
@@ -8374,12 +8471,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="T3:U3"/>
     <mergeCell ref="BD3:BE3"/>
     <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="AC3:AD3"/>
@@ -8388,6 +8479,12 @@
     <mergeCell ref="AO3:AQ3"/>
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Daily Appointment Calendar in this worksheet. Enter appointment details in Appointments table starting in cell B2" sqref="A3" xr:uid="{020C3CF3-3449-4B9F-99EF-39A67433C720}"/>
@@ -9595,12 +9692,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="T3:U3"/>
     <mergeCell ref="BD3:BE3"/>
     <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="AC3:AD3"/>
@@ -9609,6 +9700,12 @@
     <mergeCell ref="AO3:AQ3"/>
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="E4 H4 N4 Q4 W4 Z4 AF4 AI4 AO4 AR4 AX4 BA4 BG4 BJ4" xr:uid="{C256AD20-86C3-43AF-A157-F6F748ADAD93}"/>
@@ -10816,12 +10913,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="T3:U3"/>
     <mergeCell ref="BD3:BE3"/>
     <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="AC3:AD3"/>
@@ -10830,6 +10921,12 @@
     <mergeCell ref="AO3:AQ3"/>
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Daily Appointment Calendar in this worksheet. Enter appointment details in Appointments table starting in cell B2" sqref="A3" xr:uid="{D3B88787-9666-4829-AF1B-AFD0BDE5ED0F}"/>
@@ -12037,12 +12134,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="W3:Y3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="T3:U3"/>
     <mergeCell ref="BD3:BE3"/>
     <mergeCell ref="BG3:BI3"/>
     <mergeCell ref="AC3:AD3"/>
@@ -12051,6 +12142,12 @@
     <mergeCell ref="AO3:AQ3"/>
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AX3:AZ3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="E4 H4 N4 Q4 W4 Z4 AF4 AI4 AO4 AR4 AX4 BA4 BG4 BJ4" xr:uid="{5FAFC48E-2820-4639-899D-6240921BAB5B}"/>
@@ -12081,14 +12178,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="544010ab-5998-4e47-9e28-04d882867513" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100577685AB90FCC4498475D6452D048D90" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6fe2089005366a98f0abf53e193a6fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="544010ab-5998-4e47-9e28-04d882867513" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b810a13fcf3b4b751b6351b05549f6f" ns3:_="">
     <xsd:import namespace="544010ab-5998-4e47-9e28-04d882867513"/>
@@ -12278,6 +12367,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="544010ab-5998-4e47-9e28-04d882867513" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -12288,22 +12385,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78FE3DBD-4BA3-46F9-ACF1-8875F3E925DE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="544010ab-5998-4e47-9e28-04d882867513"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB62CB31-3897-439C-929D-5AFDFE1F0635}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12321,6 +12402,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78FE3DBD-4BA3-46F9-ACF1-8875F3E925DE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="544010ab-5998-4e47-9e28-04d882867513"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E7A5433-9782-480E-ABBF-A825B9458B88}">
   <ds:schemaRefs>

</xml_diff>